<commit_message>
Fix column B data validation
</commit_message>
<xml_diff>
--- a/Fabric-Nodes.xlsx
+++ b/Fabric-Nodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACI-Register-Nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6833B426-3E8F-453C-8781-17B6BD066E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6879CB-7D24-4F09-BC28-B7DFF5A97A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,12 +57,6 @@
     <t>Leaf-102</t>
   </si>
   <si>
-    <t>Spine-103</t>
-  </si>
-  <si>
-    <t>Spine-104</t>
-  </si>
-  <si>
     <t>Node Name</t>
   </si>
   <si>
@@ -79,13 +73,19 @@
   </si>
   <si>
     <t>spine</t>
+  </si>
+  <si>
+    <t>Spine-201</t>
+  </si>
+  <si>
+    <t>Spine-202</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +106,12 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -461,10 +467,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -473,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
@@ -481,10 +487,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -501,10 +507,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -521,10 +527,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -533,18 +539,18 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1">
-        <v>103</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -553,17 +559,18 @@
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
-        <v>104</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Invalid Node Type!" promptTitle="Please select a Node Type" prompt="If uncertain, select unspecified" sqref="B2:B5" xr:uid="{63D24343-A989-49A3-9651-AF8FEF5A6AFC}">
-      <formula1>"remote-leaf-wan,tier-2-leaf,unspecified,virtual"</formula1>
+      <formula1>"spine,leaf,unspecified"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5" xr:uid="{D786AEA1-2A43-40E7-AF03-F83C2A056398}">
       <formula1>"spine,leaf,unspecified"</formula1>

</xml_diff>

<commit_message>
Remove values from POD ID
</commit_message>
<xml_diff>
--- a/Fabric-Nodes.xlsx
+++ b/Fabric-Nodes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACI-Register-Nodes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevNet-Course\ACI-Course\ACI-Register-Nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6879CB-7D24-4F09-BC28-B7DFF5A97A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C0F974-F2DE-48DB-81E5-C7672C604A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fabric Nodes" sheetId="1" r:id="rId1"/>
@@ -452,7 +452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -492,9 +494,7 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
@@ -512,9 +512,7 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
@@ -532,9 +530,7 @@
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
@@ -552,9 +548,7 @@
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>